<commit_message>
without 0 rated universities
</commit_message>
<xml_diff>
--- a/data/uni.xlsx
+++ b/data/uni.xlsx
@@ -9604,8 +9604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9667,9 +9667,6 @@
       <c r="A7" t="s">
         <v>474</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -9683,9 +9680,6 @@
       <c r="A9" t="s">
         <v>476</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -9699,9 +9693,6 @@
       <c r="A11" t="s">
         <v>478</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -9742,17 +9733,11 @@
       <c r="A16" t="s">
         <v>482</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>483</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -9774,9 +9759,6 @@
       <c r="A20" t="s">
         <v>484</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -9806,9 +9788,6 @@
       <c r="A24" t="s">
         <v>487</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -9854,9 +9833,6 @@
       <c r="A30" t="s">
         <v>491</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -9974,17 +9950,11 @@
       <c r="A45" t="s">
         <v>506</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>507</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -10006,9 +9976,6 @@
       <c r="A49" t="s">
         <v>510</v>
       </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -10042,9 +10009,6 @@
       <c r="A53" t="s">
         <v>514</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -10066,9 +10030,6 @@
       <c r="A56" t="s">
         <v>517</v>
       </c>
-      <c r="B56">
-        <v>0</v>
-      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -10098,9 +10059,6 @@
       <c r="A60" t="s">
         <v>520</v>
       </c>
-      <c r="B60">
-        <v>0</v>
-      </c>
       <c r="C60" t="s">
         <v>536</v>
       </c>
@@ -10203,9 +10161,6 @@
       <c r="A72" t="s">
         <v>532</v>
       </c>
-      <c r="B72">
-        <v>0</v>
-      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -10218,9 +10173,6 @@
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>534</v>
-      </c>
-      <c r="B74">
-        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>